<commit_message>
reworked dataset and rscript, added plot pngs
</commit_message>
<xml_diff>
--- a/risultati.xlsx
+++ b/risultati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xzeni\OneDrive\Desktop\CodeSmell-DesignPattern-Experiment-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2409AF1-ABAA-457D-898D-D603E76BAC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58875307-D38E-4209-A0A7-46C663D6EBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -914,10 +914,10 @@
     <t>EM_8</t>
   </si>
   <si>
-    <t>Errate _Comprensione</t>
-  </si>
-  <si>
-    <t>Errate_Manutenzione</t>
+    <t>Rapporto_Comprensione</t>
+  </si>
+  <si>
+    <t>Rapporto_Manutenzione</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1188,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1196,12 +1195,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6843,7 +6843,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6857,76 +6857,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="O1" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="T1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="U1" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="W1" s="22" t="s">
+      <c r="W1" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="X1" s="22" t="s">
+      <c r="X1" s="21" t="s">
         <v>85</v>
       </c>
     </row>
@@ -6937,72 +6937,74 @@
       <c r="B2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="23">
         <v>6</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="19">
         <v>3</v>
       </c>
-      <c r="E2" s="28">
-        <v>2</v>
-      </c>
-      <c r="F2" s="21">
-        <v>5</v>
+      <c r="E2" s="25">
+        <f>C2/8</f>
+        <v>0.75</v>
+      </c>
+      <c r="F2" s="24">
+        <f>D2/8</f>
+        <v>0.375</v>
       </c>
       <c r="G2" s="8">
         <v>7</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2">
         <v>4</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2">
         <v>2</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2">
         <v>3</v>
       </c>
-      <c r="M2" s="15">
+      <c r="M2">
         <v>3</v>
       </c>
-      <c r="N2" s="15">
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="O2" s="16">
+      <c r="O2" s="15">
         <v>8</v>
       </c>
-      <c r="P2" s="17">
+      <c r="P2" s="16">
         <v>10</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="Q2" s="16">
         <v>5</v>
       </c>
-      <c r="R2" s="17">
+      <c r="R2" s="16">
         <v>3</v>
       </c>
-      <c r="S2" s="17">
+      <c r="S2" s="16">
         <v>12</v>
       </c>
-      <c r="T2" s="17">
+      <c r="T2" s="16">
         <v>2</v>
       </c>
-      <c r="U2" s="17">
+      <c r="U2" s="16">
         <v>2</v>
       </c>
-      <c r="V2" s="18">
+      <c r="V2" s="17">
         <v>4</v>
       </c>
-      <c r="W2" s="28">
-        <f>AVERAGE(G2:N2)</f>
+      <c r="W2" s="23">
+        <f t="shared" ref="W2:W12" si="0">AVERAGE(G2:N2)</f>
         <v>3.25</v>
       </c>
-      <c r="X2" s="28">
-        <f>AVERAGE(O2:V2)</f>
+      <c r="X2" s="23">
+        <f t="shared" ref="X2:X12" si="1">AVERAGE(O2:V2)</f>
         <v>5.75</v>
       </c>
     </row>
@@ -7016,69 +7018,71 @@
       <c r="C3" s="9">
         <v>6</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="24">
         <v>5</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="26">
+        <f t="shared" ref="E3:E12" si="2">C3/8</f>
+        <v>0.75</v>
+      </c>
+      <c r="F3" s="24">
+        <f t="shared" ref="F3:F12" si="3">D3/8</f>
+        <v>0.625</v>
+      </c>
+      <c r="G3" s="18">
+        <v>5</v>
+      </c>
+      <c r="H3" s="19">
+        <v>8</v>
+      </c>
+      <c r="I3" s="19">
+        <v>6</v>
+      </c>
+      <c r="J3" s="19">
+        <v>6</v>
+      </c>
+      <c r="K3" s="19">
         <v>2</v>
       </c>
-      <c r="F3" s="11">
+      <c r="L3" s="19">
+        <v>4</v>
+      </c>
+      <c r="M3" s="22">
         <v>3</v>
       </c>
-      <c r="G3" s="19">
+      <c r="N3" s="19">
+        <v>2</v>
+      </c>
+      <c r="O3" s="15">
         <v>5</v>
       </c>
-      <c r="H3" s="20">
-        <v>8</v>
-      </c>
-      <c r="I3" s="20">
+      <c r="P3" s="16">
+        <v>11</v>
+      </c>
+      <c r="Q3" s="16">
         <v>6</v>
       </c>
-      <c r="J3" s="20">
+      <c r="R3" s="16">
+        <v>20</v>
+      </c>
+      <c r="S3" s="16">
+        <v>2</v>
+      </c>
+      <c r="T3" s="16">
+        <v>2</v>
+      </c>
+      <c r="U3" s="16">
+        <v>3</v>
+      </c>
+      <c r="V3" s="17">
         <v>6</v>
       </c>
-      <c r="K3" s="20">
-        <v>2</v>
-      </c>
-      <c r="L3" s="20">
-        <v>4</v>
-      </c>
-      <c r="M3" s="25">
-        <v>3</v>
-      </c>
-      <c r="N3" s="20">
-        <v>2</v>
-      </c>
-      <c r="O3" s="16">
-        <v>5</v>
-      </c>
-      <c r="P3" s="17">
-        <v>11</v>
-      </c>
-      <c r="Q3" s="17">
-        <v>6</v>
-      </c>
-      <c r="R3" s="17">
-        <v>20</v>
-      </c>
-      <c r="S3" s="17">
-        <v>2</v>
-      </c>
-      <c r="T3" s="17">
-        <v>2</v>
-      </c>
-      <c r="U3" s="17">
-        <v>3</v>
-      </c>
-      <c r="V3" s="18">
-        <v>6</v>
-      </c>
       <c r="W3" s="9">
-        <f>AVERAGE(G3:N3)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="X3" s="9">
-        <f>AVERAGE(O3:V3)</f>
+        <f t="shared" si="1"/>
         <v>6.875</v>
       </c>
     </row>
@@ -7092,69 +7096,71 @@
       <c r="C4" s="9">
         <v>6</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="24">
         <v>5</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="26">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="F4" s="24">
+        <f t="shared" si="3"/>
+        <v>0.625</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1</v>
+      </c>
+      <c r="H4" s="16">
+        <v>17</v>
+      </c>
+      <c r="I4" s="16">
+        <v>3</v>
+      </c>
+      <c r="J4" s="16">
+        <v>11</v>
+      </c>
+      <c r="K4" s="16">
+        <v>1</v>
+      </c>
+      <c r="L4" s="16">
+        <v>1</v>
+      </c>
+      <c r="M4" s="16">
+        <v>1</v>
+      </c>
+      <c r="N4" s="16">
+        <v>1</v>
+      </c>
+      <c r="O4" s="15">
+        <v>8</v>
+      </c>
+      <c r="P4" s="16">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="16">
+        <v>6</v>
+      </c>
+      <c r="R4" s="16">
+        <v>3</v>
+      </c>
+      <c r="S4" s="16">
         <v>2</v>
       </c>
-      <c r="F4" s="11">
-        <v>3</v>
-      </c>
-      <c r="G4" s="16">
+      <c r="T4" s="16">
+        <v>4</v>
+      </c>
+      <c r="U4" s="16">
         <v>1</v>
       </c>
-      <c r="H4" s="17">
-        <v>17</v>
-      </c>
-      <c r="I4" s="17">
-        <v>3</v>
-      </c>
-      <c r="J4" s="17">
-        <v>11</v>
-      </c>
-      <c r="K4" s="17">
+      <c r="V4" s="17">
         <v>1</v>
       </c>
-      <c r="L4" s="17">
-        <v>1</v>
-      </c>
-      <c r="M4" s="17">
-        <v>1</v>
-      </c>
-      <c r="N4" s="17">
-        <v>1</v>
-      </c>
-      <c r="O4" s="16">
-        <v>8</v>
-      </c>
-      <c r="P4" s="17">
-        <v>16</v>
-      </c>
-      <c r="Q4" s="17">
-        <v>6</v>
-      </c>
-      <c r="R4" s="17">
-        <v>3</v>
-      </c>
-      <c r="S4" s="17">
-        <v>2</v>
-      </c>
-      <c r="T4" s="17">
-        <v>4</v>
-      </c>
-      <c r="U4" s="17">
-        <v>1</v>
-      </c>
-      <c r="V4" s="18">
-        <v>1</v>
-      </c>
       <c r="W4" s="9">
-        <f>AVERAGE(G4:N4)</f>
+        <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="X4" s="9">
-        <f>AVERAGE(O4:V4)</f>
+        <f t="shared" si="1"/>
         <v>5.125</v>
       </c>
     </row>
@@ -7168,69 +7174,71 @@
       <c r="C5" s="9">
         <v>5</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="24">
         <v>4</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="26">
+        <f t="shared" si="2"/>
+        <v>0.625</v>
+      </c>
+      <c r="F5" s="24">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="15">
+        <v>12</v>
+      </c>
+      <c r="H5" s="16">
+        <v>10</v>
+      </c>
+      <c r="I5" s="16">
+        <v>10</v>
+      </c>
+      <c r="J5" s="16">
+        <v>6</v>
+      </c>
+      <c r="K5" s="16">
+        <v>1</v>
+      </c>
+      <c r="L5" s="16">
+        <v>4</v>
+      </c>
+      <c r="M5" s="16">
+        <v>5</v>
+      </c>
+      <c r="N5" s="16">
+        <v>1</v>
+      </c>
+      <c r="O5" s="15">
+        <v>4</v>
+      </c>
+      <c r="P5" s="16">
+        <v>6</v>
+      </c>
+      <c r="Q5" s="16">
+        <v>6</v>
+      </c>
+      <c r="R5" s="16">
         <v>3</v>
       </c>
-      <c r="F5" s="11">
-        <v>4</v>
-      </c>
-      <c r="G5" s="16">
-        <v>12</v>
-      </c>
-      <c r="H5" s="17">
-        <v>10</v>
-      </c>
-      <c r="I5" s="17">
-        <v>10</v>
-      </c>
-      <c r="J5" s="17">
-        <v>6</v>
-      </c>
-      <c r="K5" s="17">
+      <c r="S5" s="16">
+        <v>3</v>
+      </c>
+      <c r="T5" s="16">
+        <v>2</v>
+      </c>
+      <c r="U5" s="16">
         <v>1</v>
       </c>
-      <c r="L5" s="17">
-        <v>4</v>
-      </c>
-      <c r="M5" s="17">
-        <v>5</v>
-      </c>
-      <c r="N5" s="17">
-        <v>1</v>
-      </c>
-      <c r="O5" s="16">
-        <v>4</v>
-      </c>
-      <c r="P5" s="17">
-        <v>6</v>
-      </c>
-      <c r="Q5" s="17">
-        <v>6</v>
-      </c>
-      <c r="R5" s="17">
+      <c r="V5" s="17">
         <v>3</v>
       </c>
-      <c r="S5" s="17">
-        <v>3</v>
-      </c>
-      <c r="T5" s="17">
-        <v>2</v>
-      </c>
-      <c r="U5" s="17">
-        <v>1</v>
-      </c>
-      <c r="V5" s="18">
-        <v>3</v>
-      </c>
       <c r="W5" s="9">
-        <f>AVERAGE(G5:N5)</f>
+        <f t="shared" si="0"/>
         <v>6.125</v>
       </c>
       <c r="X5" s="9">
-        <f>AVERAGE(O5:V5)</f>
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
@@ -7244,69 +7252,71 @@
       <c r="C6" s="9">
         <v>5</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="24">
         <v>6</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="26">
+        <f t="shared" si="2"/>
+        <v>0.625</v>
+      </c>
+      <c r="F6" s="24">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="G6" s="15">
+        <v>10</v>
+      </c>
+      <c r="H6" s="16">
+        <v>14</v>
+      </c>
+      <c r="I6" s="16">
+        <v>17</v>
+      </c>
+      <c r="J6" s="16">
         <v>3</v>
       </c>
-      <c r="F6" s="11">
+      <c r="K6" s="16">
         <v>2</v>
       </c>
-      <c r="G6" s="16">
-        <v>10</v>
-      </c>
-      <c r="H6" s="17">
-        <v>14</v>
-      </c>
-      <c r="I6" s="17">
-        <v>17</v>
-      </c>
-      <c r="J6" s="17">
+      <c r="L6" s="16">
+        <v>4</v>
+      </c>
+      <c r="M6" s="16">
+        <v>4</v>
+      </c>
+      <c r="N6" s="16">
+        <v>5</v>
+      </c>
+      <c r="O6" s="15">
+        <v>11</v>
+      </c>
+      <c r="P6" s="16">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="16">
+        <v>8</v>
+      </c>
+      <c r="R6" s="16">
         <v>3</v>
       </c>
-      <c r="K6" s="17">
+      <c r="S6" s="16">
+        <v>3</v>
+      </c>
+      <c r="T6" s="16">
+        <v>3</v>
+      </c>
+      <c r="U6" s="16">
         <v>2</v>
       </c>
-      <c r="L6" s="17">
+      <c r="V6" s="17">
         <v>4</v>
       </c>
-      <c r="M6" s="17">
-        <v>4</v>
-      </c>
-      <c r="N6" s="17">
-        <v>5</v>
-      </c>
-      <c r="O6" s="16">
-        <v>11</v>
-      </c>
-      <c r="P6" s="17">
-        <v>18</v>
-      </c>
-      <c r="Q6" s="17">
-        <v>8</v>
-      </c>
-      <c r="R6" s="17">
-        <v>3</v>
-      </c>
-      <c r="S6" s="17">
-        <v>3</v>
-      </c>
-      <c r="T6" s="17">
-        <v>3</v>
-      </c>
-      <c r="U6" s="17">
-        <v>2</v>
-      </c>
-      <c r="V6" s="18">
-        <v>4</v>
-      </c>
       <c r="W6" s="9">
-        <f>AVERAGE(G6:N6)</f>
+        <f t="shared" si="0"/>
         <v>7.375</v>
       </c>
       <c r="X6" s="9">
-        <f>AVERAGE(O6:V6)</f>
+        <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
     </row>
@@ -7320,69 +7330,71 @@
       <c r="C7" s="9">
         <v>6</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="24">
         <v>5</v>
       </c>
-      <c r="E7" s="9">
-        <v>2</v>
-      </c>
-      <c r="F7" s="11">
-        <v>3</v>
+      <c r="E7" s="26">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="F7" s="24">
+        <f t="shared" si="3"/>
+        <v>0.625</v>
       </c>
       <c r="G7" s="8">
         <v>2</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7">
         <v>7</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7">
         <v>3</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7">
         <v>4</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7">
         <v>2</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7">
         <v>2</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7">
         <v>2</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7">
         <v>2</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="18">
         <v>10</v>
       </c>
-      <c r="P7" s="20">
+      <c r="P7" s="19">
         <v>4</v>
       </c>
-      <c r="Q7" s="20">
+      <c r="Q7" s="19">
         <v>4</v>
       </c>
-      <c r="R7" s="20">
+      <c r="R7" s="19">
         <v>3</v>
       </c>
-      <c r="S7" s="20">
+      <c r="S7" s="19">
         <v>14</v>
       </c>
-      <c r="T7" s="20">
+      <c r="T7" s="19">
         <v>2</v>
       </c>
-      <c r="U7" s="20">
+      <c r="U7" s="19">
         <v>2</v>
       </c>
-      <c r="V7" s="21">
+      <c r="V7" s="20">
         <v>3</v>
       </c>
       <c r="W7" s="9">
-        <f>AVERAGE(G7:N7)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="X7" s="9">
-        <f>AVERAGE(O7:V7)</f>
+        <f t="shared" si="1"/>
         <v>5.25</v>
       </c>
     </row>
@@ -7396,69 +7408,71 @@
       <c r="C8" s="9">
         <v>8</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="24">
         <v>7</v>
       </c>
-      <c r="E8" s="9">
-        <v>0</v>
-      </c>
-      <c r="F8" s="11">
+      <c r="E8" s="26">
+        <f>C8/8</f>
         <v>1</v>
       </c>
-      <c r="G8" s="16">
+      <c r="F8" s="24">
+        <f t="shared" si="3"/>
+        <v>0.875</v>
+      </c>
+      <c r="G8" s="15">
         <v>1</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <v>1</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <v>1</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="16">
         <v>1</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="16">
         <v>1</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>1</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="16">
         <v>4</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="16">
         <v>5</v>
       </c>
-      <c r="O8" s="16">
+      <c r="O8" s="15">
         <v>1</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="16">
         <v>1</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="16">
         <v>2</v>
       </c>
-      <c r="R8" s="17">
+      <c r="R8" s="16">
         <v>1</v>
       </c>
-      <c r="S8" s="17">
+      <c r="S8" s="16">
         <v>4</v>
       </c>
-      <c r="T8" s="17">
+      <c r="T8" s="16">
         <v>4</v>
       </c>
-      <c r="U8" s="17">
+      <c r="U8" s="16">
         <v>3</v>
       </c>
-      <c r="V8" s="18">
+      <c r="V8" s="17">
         <v>7</v>
       </c>
       <c r="W8" s="9">
-        <f>AVERAGE(G8:N8)</f>
+        <f t="shared" si="0"/>
         <v>1.875</v>
       </c>
       <c r="X8" s="9">
-        <f>AVERAGE(O8:V8)</f>
+        <f t="shared" si="1"/>
         <v>2.875</v>
       </c>
     </row>
@@ -7472,69 +7486,71 @@
       <c r="C9" s="9">
         <v>7</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="24">
         <v>3</v>
       </c>
-      <c r="E9" s="9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11">
+      <c r="E9" s="26">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+      <c r="F9" s="24">
+        <f t="shared" si="3"/>
+        <v>0.375</v>
+      </c>
+      <c r="G9" s="15">
+        <v>4</v>
+      </c>
+      <c r="H9" s="16">
+        <v>3</v>
+      </c>
+      <c r="I9" s="16">
+        <v>2</v>
+      </c>
+      <c r="J9" s="16">
+        <v>3</v>
+      </c>
+      <c r="K9" s="16">
+        <v>2</v>
+      </c>
+      <c r="L9" s="16">
+        <v>2</v>
+      </c>
+      <c r="M9" s="16">
+        <v>2</v>
+      </c>
+      <c r="N9" s="16">
+        <v>3</v>
+      </c>
+      <c r="O9" s="15">
+        <v>12</v>
+      </c>
+      <c r="P9" s="16">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="16">
+        <v>8</v>
+      </c>
+      <c r="R9" s="16">
+        <v>7</v>
+      </c>
+      <c r="S9" s="16">
+        <v>8</v>
+      </c>
+      <c r="T9" s="16">
         <v>5</v>
       </c>
-      <c r="G9" s="16">
-        <v>4</v>
-      </c>
-      <c r="H9" s="17">
+      <c r="U9" s="16">
+        <v>8</v>
+      </c>
+      <c r="V9" s="17">
         <v>3</v>
       </c>
-      <c r="I9" s="17">
-        <v>2</v>
-      </c>
-      <c r="J9" s="17">
-        <v>3</v>
-      </c>
-      <c r="K9" s="17">
-        <v>2</v>
-      </c>
-      <c r="L9" s="17">
-        <v>2</v>
-      </c>
-      <c r="M9" s="17">
-        <v>2</v>
-      </c>
-      <c r="N9" s="17">
-        <v>3</v>
-      </c>
-      <c r="O9" s="16">
-        <v>12</v>
-      </c>
-      <c r="P9" s="17">
-        <v>4</v>
-      </c>
-      <c r="Q9" s="17">
-        <v>8</v>
-      </c>
-      <c r="R9" s="17">
-        <v>7</v>
-      </c>
-      <c r="S9" s="17">
-        <v>8</v>
-      </c>
-      <c r="T9" s="17">
-        <v>5</v>
-      </c>
-      <c r="U9" s="17">
-        <v>8</v>
-      </c>
-      <c r="V9" s="18">
-        <v>3</v>
-      </c>
       <c r="W9" s="9">
-        <f>AVERAGE(G9:N9)</f>
+        <f t="shared" si="0"/>
         <v>2.625</v>
       </c>
       <c r="X9" s="9">
-        <f>AVERAGE(O9:V9)</f>
+        <f t="shared" si="1"/>
         <v>6.875</v>
       </c>
     </row>
@@ -7548,69 +7564,71 @@
       <c r="C10" s="9">
         <v>7</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="24">
         <v>7</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="26">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+      <c r="F10" s="24">
+        <f t="shared" si="3"/>
+        <v>0.875</v>
+      </c>
+      <c r="G10" s="15">
+        <v>2</v>
+      </c>
+      <c r="H10" s="16">
+        <v>2</v>
+      </c>
+      <c r="I10" s="16">
+        <v>2</v>
+      </c>
+      <c r="J10" s="16">
+        <v>2</v>
+      </c>
+      <c r="K10" s="16">
         <v>1</v>
       </c>
-      <c r="F10" s="11">
-        <v>1</v>
-      </c>
-      <c r="G10" s="16">
-        <v>2</v>
-      </c>
-      <c r="H10" s="17">
-        <v>2</v>
-      </c>
-      <c r="I10" s="17">
-        <v>2</v>
-      </c>
-      <c r="J10" s="17">
-        <v>2</v>
-      </c>
-      <c r="K10" s="17">
-        <v>1</v>
-      </c>
-      <c r="L10" s="17">
+      <c r="L10" s="16">
         <v>3</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="16">
         <v>3</v>
       </c>
-      <c r="N10" s="17">
+      <c r="N10" s="16">
         <v>5</v>
       </c>
-      <c r="O10" s="16">
+      <c r="O10" s="15">
         <v>5</v>
       </c>
-      <c r="P10" s="17">
+      <c r="P10" s="16">
         <v>3</v>
       </c>
-      <c r="Q10" s="17">
+      <c r="Q10" s="16">
         <v>3</v>
       </c>
-      <c r="R10" s="17">
+      <c r="R10" s="16">
         <v>3</v>
       </c>
-      <c r="S10" s="17">
+      <c r="S10" s="16">
         <v>5</v>
       </c>
-      <c r="T10" s="17">
+      <c r="T10" s="16">
         <v>4</v>
       </c>
-      <c r="U10" s="17">
+      <c r="U10" s="16">
         <v>3</v>
       </c>
-      <c r="V10" s="18">
+      <c r="V10" s="17">
         <v>5</v>
       </c>
       <c r="W10" s="9">
-        <f>AVERAGE(G10:N10)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="X10" s="9">
-        <f>AVERAGE(O10:V10)</f>
+        <f t="shared" si="1"/>
         <v>3.875</v>
       </c>
     </row>
@@ -7624,69 +7642,71 @@
       <c r="C11" s="9">
         <v>7</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="24">
         <v>6</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="26">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+      <c r="F11" s="24">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="15">
+        <v>6</v>
+      </c>
+      <c r="H11" s="16">
+        <v>2</v>
+      </c>
+      <c r="I11" s="16">
+        <v>2</v>
+      </c>
+      <c r="J11" s="16">
         <v>1</v>
       </c>
-      <c r="F11" s="11">
+      <c r="K11" s="16">
+        <v>11</v>
+      </c>
+      <c r="L11" s="16">
+        <v>3</v>
+      </c>
+      <c r="M11" s="16">
         <v>2</v>
       </c>
-      <c r="G11" s="16">
-        <v>6</v>
-      </c>
-      <c r="H11" s="17">
+      <c r="N11" s="16">
+        <v>3</v>
+      </c>
+      <c r="O11" s="15">
+        <v>4</v>
+      </c>
+      <c r="P11" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>3</v>
+      </c>
+      <c r="R11" s="16">
+        <v>5</v>
+      </c>
+      <c r="S11" s="16">
+        <v>5</v>
+      </c>
+      <c r="T11" s="16">
         <v>2</v>
       </c>
-      <c r="I11" s="17">
+      <c r="U11" s="16">
+        <v>3</v>
+      </c>
+      <c r="V11" s="17">
         <v>2</v>
       </c>
-      <c r="J11" s="17">
-        <v>1</v>
-      </c>
-      <c r="K11" s="17">
-        <v>11</v>
-      </c>
-      <c r="L11" s="17">
-        <v>3</v>
-      </c>
-      <c r="M11" s="17">
-        <v>2</v>
-      </c>
-      <c r="N11" s="17">
-        <v>3</v>
-      </c>
-      <c r="O11" s="16">
-        <v>4</v>
-      </c>
-      <c r="P11" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="17">
-        <v>3</v>
-      </c>
-      <c r="R11" s="17">
-        <v>5</v>
-      </c>
-      <c r="S11" s="17">
-        <v>5</v>
-      </c>
-      <c r="T11" s="17">
-        <v>2</v>
-      </c>
-      <c r="U11" s="17">
-        <v>3</v>
-      </c>
-      <c r="V11" s="18">
-        <v>2</v>
-      </c>
       <c r="W11" s="9">
-        <f>AVERAGE(G11:N11)</f>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
       <c r="X11" s="9">
-        <f>AVERAGE(O11:V11)</f>
+        <f t="shared" si="1"/>
         <v>3.125</v>
       </c>
     </row>
@@ -7700,69 +7720,71 @@
       <c r="C12" s="9">
         <v>7</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="24">
         <v>4</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="26">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+      <c r="F12" s="24">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="18">
+        <v>12</v>
+      </c>
+      <c r="H12" s="19">
+        <v>7</v>
+      </c>
+      <c r="I12" s="19">
+        <v>7</v>
+      </c>
+      <c r="J12" s="19">
+        <v>10</v>
+      </c>
+      <c r="K12" s="19">
+        <v>2</v>
+      </c>
+      <c r="L12" s="19">
+        <v>2</v>
+      </c>
+      <c r="M12" s="19">
         <v>1</v>
       </c>
-      <c r="F12" s="11">
+      <c r="N12" s="19">
+        <v>3</v>
+      </c>
+      <c r="O12" s="18">
+        <v>12</v>
+      </c>
+      <c r="P12" s="19">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>9</v>
+      </c>
+      <c r="R12" s="19">
+        <v>6</v>
+      </c>
+      <c r="S12" s="19">
         <v>4</v>
       </c>
-      <c r="G12" s="19">
-        <v>12</v>
-      </c>
-      <c r="H12" s="20">
-        <v>7</v>
-      </c>
-      <c r="I12" s="20">
-        <v>7</v>
-      </c>
-      <c r="J12" s="20">
-        <v>10</v>
-      </c>
-      <c r="K12" s="20">
+      <c r="T12" s="19">
+        <v>6</v>
+      </c>
+      <c r="U12" s="19">
+        <v>3</v>
+      </c>
+      <c r="V12" s="20">
         <v>2</v>
       </c>
-      <c r="L12" s="20">
-        <v>2</v>
-      </c>
-      <c r="M12" s="20">
-        <v>1</v>
-      </c>
-      <c r="N12" s="20">
-        <v>3</v>
-      </c>
-      <c r="O12" s="19">
-        <v>12</v>
-      </c>
-      <c r="P12" s="20">
-        <v>6</v>
-      </c>
-      <c r="Q12" s="20">
-        <v>9</v>
-      </c>
-      <c r="R12" s="20">
-        <v>6</v>
-      </c>
-      <c r="S12" s="20">
-        <v>4</v>
-      </c>
-      <c r="T12" s="20">
-        <v>6</v>
-      </c>
-      <c r="U12" s="20">
-        <v>3</v>
-      </c>
-      <c r="V12" s="21">
-        <v>2</v>
-      </c>
       <c r="W12" s="9">
-        <f>AVERAGE(G12:N12)</f>
+        <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
       <c r="X12" s="9">
-        <f>AVERAGE(O12:V12)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -7776,59 +7798,61 @@
       <c r="C13" s="9">
         <v>5</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="24">
         <v>7</v>
       </c>
       <c r="E13" s="9">
+        <f>C13/7</f>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="F13" s="27">
+        <f>D13/7</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="15">
         <v>2</v>
       </c>
-      <c r="F13" s="11">
-        <v>0</v>
-      </c>
-      <c r="G13" s="16">
+      <c r="H13" s="16">
         <v>2</v>
       </c>
-      <c r="H13" s="17">
+      <c r="I13" s="16">
+        <v>4</v>
+      </c>
+      <c r="J13" s="16">
         <v>2</v>
       </c>
-      <c r="I13" s="17">
+      <c r="K13" s="16">
         <v>4</v>
       </c>
-      <c r="J13" s="17">
+      <c r="L13" s="16">
+        <v>6</v>
+      </c>
+      <c r="M13" s="16">
         <v>2</v>
       </c>
-      <c r="K13" s="17">
+      <c r="N13" s="16"/>
+      <c r="O13" s="15">
+        <v>5</v>
+      </c>
+      <c r="P13" s="16">
+        <v>5</v>
+      </c>
+      <c r="Q13" s="16">
+        <v>5</v>
+      </c>
+      <c r="R13" s="16">
+        <v>5</v>
+      </c>
+      <c r="S13" s="16">
+        <v>5</v>
+      </c>
+      <c r="T13" s="16">
         <v>4</v>
       </c>
-      <c r="L13" s="17">
-        <v>6</v>
-      </c>
-      <c r="M13" s="17">
-        <v>2</v>
-      </c>
-      <c r="N13" s="17"/>
-      <c r="O13" s="16">
-        <v>5</v>
-      </c>
-      <c r="P13" s="17">
-        <v>5</v>
-      </c>
-      <c r="Q13" s="17">
-        <v>5</v>
-      </c>
-      <c r="R13" s="17">
-        <v>5</v>
-      </c>
-      <c r="S13" s="17">
-        <v>5</v>
-      </c>
-      <c r="T13" s="17">
-        <v>4</v>
-      </c>
-      <c r="U13" s="17">
+      <c r="U13" s="16">
         <v>3</v>
       </c>
-      <c r="V13" s="18"/>
+      <c r="V13" s="17"/>
       <c r="W13" s="9">
         <f>AVERAGE(G13:M13)</f>
         <v>3.1428571428571428</v>
@@ -7848,59 +7872,61 @@
       <c r="C14" s="9">
         <v>6</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="24">
         <v>7</v>
       </c>
       <c r="E14" s="9">
+        <f t="shared" ref="E14:E16" si="4">C14/7</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="F14" s="27">
+        <f t="shared" ref="F14:F16" si="5">D14/7</f>
         <v>1</v>
       </c>
-      <c r="F14" s="11">
-        <v>0</v>
-      </c>
-      <c r="G14" s="16">
+      <c r="G14" s="15">
         <v>5</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="16">
         <v>1</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="16">
         <v>7</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="16">
         <v>2</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="16">
         <v>1</v>
       </c>
-      <c r="L14" s="17">
+      <c r="L14" s="16">
         <v>3</v>
       </c>
-      <c r="M14" s="17">
+      <c r="M14" s="16">
         <v>4</v>
       </c>
-      <c r="N14" s="17"/>
-      <c r="O14" s="16">
+      <c r="N14" s="16"/>
+      <c r="O14" s="15">
         <v>5</v>
       </c>
-      <c r="P14" s="17">
+      <c r="P14" s="16">
         <v>3</v>
       </c>
-      <c r="Q14" s="17">
+      <c r="Q14" s="16">
         <v>4</v>
       </c>
-      <c r="R14" s="17">
+      <c r="R14" s="16">
         <v>4</v>
       </c>
-      <c r="S14" s="17">
+      <c r="S14" s="16">
         <v>4</v>
       </c>
-      <c r="T14" s="17">
+      <c r="T14" s="16">
         <v>3</v>
       </c>
-      <c r="U14" s="17">
+      <c r="U14" s="16">
         <v>4</v>
       </c>
-      <c r="V14" s="18"/>
+      <c r="V14" s="17"/>
       <c r="W14" s="9">
         <f>AVERAGE(G14:M14)</f>
         <v>3.2857142857142856</v>
@@ -7920,59 +7946,61 @@
       <c r="C15" s="9">
         <v>6</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="24">
         <v>7</v>
       </c>
       <c r="E15" s="9">
+        <f t="shared" si="4"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="F15" s="27">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="F15" s="11">
-        <v>0</v>
-      </c>
-      <c r="G15" s="16">
+      <c r="G15" s="15">
         <v>3</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="16">
         <v>3</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="16">
         <v>5</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="16">
         <v>1</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="16">
         <v>1</v>
       </c>
-      <c r="L15" s="17">
+      <c r="L15" s="16">
         <v>5</v>
       </c>
-      <c r="M15" s="17">
+      <c r="M15" s="16">
         <v>1</v>
       </c>
-      <c r="N15" s="17"/>
-      <c r="O15" s="16">
+      <c r="N15" s="16"/>
+      <c r="O15" s="15">
         <v>4</v>
       </c>
-      <c r="P15" s="17">
+      <c r="P15" s="16">
         <v>5</v>
       </c>
-      <c r="Q15" s="17">
+      <c r="Q15" s="16">
         <v>7</v>
       </c>
-      <c r="R15" s="17">
+      <c r="R15" s="16">
         <v>2</v>
       </c>
-      <c r="S15" s="17">
+      <c r="S15" s="16">
         <v>2</v>
       </c>
-      <c r="T15" s="17">
+      <c r="T15" s="16">
         <v>15</v>
       </c>
-      <c r="U15" s="17">
+      <c r="U15" s="16">
         <v>1</v>
       </c>
-      <c r="V15" s="18"/>
+      <c r="V15" s="17"/>
       <c r="W15" s="9">
         <f>AVERAGE(G15:M15)</f>
         <v>2.7142857142857144</v>
@@ -7992,59 +8020,61 @@
       <c r="C16" s="9">
         <v>7</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="24">
         <v>5</v>
       </c>
       <c r="E16" s="9">
-        <v>0</v>
-      </c>
-      <c r="F16" s="11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="27">
+        <f t="shared" si="5"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="G16" s="18">
+        <v>1</v>
+      </c>
+      <c r="H16" s="19">
         <v>2</v>
       </c>
-      <c r="G16" s="19">
+      <c r="I16" s="19">
         <v>1</v>
       </c>
-      <c r="H16" s="20">
+      <c r="J16" s="19">
+        <v>1</v>
+      </c>
+      <c r="K16" s="19">
+        <v>1</v>
+      </c>
+      <c r="L16" s="19">
+        <v>1</v>
+      </c>
+      <c r="M16" s="19">
+        <v>1</v>
+      </c>
+      <c r="N16" s="19"/>
+      <c r="O16" s="18">
+        <v>3</v>
+      </c>
+      <c r="P16" s="19">
         <v>2</v>
       </c>
-      <c r="I16" s="20">
+      <c r="Q16" s="19">
+        <v>4</v>
+      </c>
+      <c r="R16" s="19">
         <v>1</v>
       </c>
-      <c r="J16" s="20">
+      <c r="S16" s="19">
+        <v>2</v>
+      </c>
+      <c r="T16" s="19">
+        <v>2</v>
+      </c>
+      <c r="U16" s="19">
         <v>1</v>
       </c>
-      <c r="K16" s="20">
-        <v>1</v>
-      </c>
-      <c r="L16" s="20">
-        <v>1</v>
-      </c>
-      <c r="M16" s="20">
-        <v>1</v>
-      </c>
-      <c r="N16" s="20"/>
-      <c r="O16" s="19">
-        <v>3</v>
-      </c>
-      <c r="P16" s="20">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="20">
-        <v>4</v>
-      </c>
-      <c r="R16" s="20">
-        <v>1</v>
-      </c>
-      <c r="S16" s="20">
-        <v>2</v>
-      </c>
-      <c r="T16" s="20">
-        <v>2</v>
-      </c>
-      <c r="U16" s="20">
-        <v>1</v>
-      </c>
-      <c r="V16" s="21"/>
+      <c r="V16" s="20"/>
       <c r="W16" s="9">
         <f>AVERAGE(G16:M16)</f>
         <v>1.1428571428571428</v>
@@ -8064,61 +8094,63 @@
       <c r="C17" s="9">
         <v>7</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="24">
         <v>6</v>
       </c>
       <c r="E17" s="9">
-        <v>1</v>
-      </c>
-      <c r="F17" s="11">
+        <f>C17/8</f>
+        <v>0.875</v>
+      </c>
+      <c r="F17" s="27">
+        <f>D17/8</f>
+        <v>0.75</v>
+      </c>
+      <c r="G17" s="15">
+        <v>9</v>
+      </c>
+      <c r="H17" s="16">
+        <v>10</v>
+      </c>
+      <c r="I17" s="16">
+        <v>14</v>
+      </c>
+      <c r="J17" s="16">
+        <v>10</v>
+      </c>
+      <c r="K17" s="16">
+        <v>4</v>
+      </c>
+      <c r="L17" s="16">
+        <v>3</v>
+      </c>
+      <c r="M17" s="16">
+        <v>3</v>
+      </c>
+      <c r="N17" s="16">
+        <v>5</v>
+      </c>
+      <c r="O17" s="15">
+        <v>3</v>
+      </c>
+      <c r="P17" s="16">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="16">
+        <v>4</v>
+      </c>
+      <c r="R17" s="16">
         <v>2</v>
       </c>
-      <c r="G17" s="16">
-        <v>9</v>
-      </c>
-      <c r="H17" s="17">
-        <v>10</v>
-      </c>
-      <c r="I17" s="17">
-        <v>14</v>
-      </c>
-      <c r="J17" s="17">
-        <v>10</v>
-      </c>
-      <c r="K17" s="17">
-        <v>4</v>
-      </c>
-      <c r="L17" s="17">
-        <v>3</v>
-      </c>
-      <c r="M17" s="17">
-        <v>3</v>
-      </c>
-      <c r="N17" s="17">
-        <v>5</v>
-      </c>
-      <c r="O17" s="16">
-        <v>3</v>
-      </c>
-      <c r="P17" s="17">
-        <v>5</v>
-      </c>
-      <c r="Q17" s="17">
-        <v>4</v>
-      </c>
-      <c r="R17" s="17">
+      <c r="S17" s="16">
         <v>2</v>
       </c>
-      <c r="S17" s="17">
+      <c r="T17" s="16">
         <v>2</v>
       </c>
-      <c r="T17" s="17">
+      <c r="U17" s="16">
         <v>2</v>
       </c>
-      <c r="U17" s="17">
-        <v>2</v>
-      </c>
-      <c r="V17" s="18">
+      <c r="V17" s="17">
         <v>2</v>
       </c>
       <c r="W17" s="9">
@@ -8140,61 +8172,63 @@
       <c r="C18" s="9">
         <v>4</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="24">
         <v>7</v>
       </c>
       <c r="E18" s="9">
+        <f t="shared" ref="E18:E21" si="6">C18/8</f>
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="27">
+        <f t="shared" ref="F18:F21" si="7">D18/8</f>
+        <v>0.875</v>
+      </c>
+      <c r="G18" s="15">
+        <v>7</v>
+      </c>
+      <c r="H18" s="16">
+        <v>3</v>
+      </c>
+      <c r="I18" s="16">
+        <v>3</v>
+      </c>
+      <c r="J18" s="16">
+        <v>3</v>
+      </c>
+      <c r="K18" s="16">
+        <v>2</v>
+      </c>
+      <c r="L18" s="16">
+        <v>3</v>
+      </c>
+      <c r="M18" s="16">
         <v>4</v>
       </c>
-      <c r="F18" s="11">
+      <c r="N18" s="16">
         <v>1</v>
       </c>
-      <c r="G18" s="16">
-        <v>7</v>
-      </c>
-      <c r="H18" s="17">
+      <c r="O18" s="15">
+        <v>5</v>
+      </c>
+      <c r="P18" s="16">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="16">
+        <v>4</v>
+      </c>
+      <c r="R18" s="16">
         <v>3</v>
       </c>
-      <c r="I18" s="17">
-        <v>3</v>
-      </c>
-      <c r="J18" s="17">
-        <v>3</v>
-      </c>
-      <c r="K18" s="17">
-        <v>2</v>
-      </c>
-      <c r="L18" s="17">
-        <v>3</v>
-      </c>
-      <c r="M18" s="17">
+      <c r="S18" s="16">
+        <v>1</v>
+      </c>
+      <c r="T18" s="16">
         <v>4</v>
       </c>
-      <c r="N18" s="17">
+      <c r="U18" s="16">
         <v>1</v>
       </c>
-      <c r="O18" s="16">
-        <v>5</v>
-      </c>
-      <c r="P18" s="17">
-        <v>4</v>
-      </c>
-      <c r="Q18" s="17">
-        <v>4</v>
-      </c>
-      <c r="R18" s="17">
-        <v>3</v>
-      </c>
-      <c r="S18" s="17">
-        <v>1</v>
-      </c>
-      <c r="T18" s="17">
-        <v>4</v>
-      </c>
-      <c r="U18" s="17">
-        <v>1</v>
-      </c>
-      <c r="V18" s="18">
+      <c r="V18" s="17">
         <v>4</v>
       </c>
       <c r="W18" s="9">
@@ -8216,61 +8250,63 @@
       <c r="C19" s="9">
         <v>5</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="24">
         <v>7</v>
       </c>
       <c r="E19" s="9">
+        <f t="shared" si="6"/>
+        <v>0.625</v>
+      </c>
+      <c r="F19" s="27">
+        <f t="shared" si="7"/>
+        <v>0.875</v>
+      </c>
+      <c r="G19" s="15">
+        <v>25</v>
+      </c>
+      <c r="H19" s="16">
+        <v>20</v>
+      </c>
+      <c r="I19" s="16">
+        <v>9</v>
+      </c>
+      <c r="J19" s="16">
+        <v>13</v>
+      </c>
+      <c r="K19" s="16">
+        <v>6</v>
+      </c>
+      <c r="L19" s="16">
         <v>3</v>
       </c>
-      <c r="F19" s="11">
+      <c r="M19" s="16">
+        <v>3</v>
+      </c>
+      <c r="N19" s="16">
+        <v>2</v>
+      </c>
+      <c r="O19" s="15">
+        <v>5</v>
+      </c>
+      <c r="P19" s="16">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="16">
+        <v>2</v>
+      </c>
+      <c r="R19" s="16">
+        <v>3</v>
+      </c>
+      <c r="S19" s="16">
+        <v>6</v>
+      </c>
+      <c r="T19" s="16">
+        <v>3</v>
+      </c>
+      <c r="U19" s="16">
         <v>1</v>
       </c>
-      <c r="G19" s="16">
-        <v>25</v>
-      </c>
-      <c r="H19" s="17">
-        <v>20</v>
-      </c>
-      <c r="I19" s="17">
-        <v>9</v>
-      </c>
-      <c r="J19" s="17">
-        <v>13</v>
-      </c>
-      <c r="K19" s="17">
-        <v>6</v>
-      </c>
-      <c r="L19" s="17">
-        <v>3</v>
-      </c>
-      <c r="M19" s="17">
-        <v>3</v>
-      </c>
-      <c r="N19" s="17">
-        <v>2</v>
-      </c>
-      <c r="O19" s="16">
-        <v>5</v>
-      </c>
-      <c r="P19" s="17">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="17">
-        <v>2</v>
-      </c>
-      <c r="R19" s="17">
-        <v>3</v>
-      </c>
-      <c r="S19" s="17">
-        <v>6</v>
-      </c>
-      <c r="T19" s="17">
-        <v>3</v>
-      </c>
-      <c r="U19" s="17">
-        <v>1</v>
-      </c>
-      <c r="V19" s="18">
+      <c r="V19" s="17">
         <v>2</v>
       </c>
       <c r="W19" s="9">
@@ -8292,61 +8328,63 @@
       <c r="C20" s="9">
         <v>6</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="24">
         <v>7</v>
       </c>
       <c r="E20" s="9">
+        <f t="shared" si="6"/>
+        <v>0.75</v>
+      </c>
+      <c r="F20" s="27">
+        <f t="shared" si="7"/>
+        <v>0.875</v>
+      </c>
+      <c r="G20" s="15">
+        <v>5</v>
+      </c>
+      <c r="H20" s="16">
+        <v>3</v>
+      </c>
+      <c r="I20" s="16">
         <v>2</v>
       </c>
-      <c r="F20" s="11">
+      <c r="J20" s="16">
+        <v>5</v>
+      </c>
+      <c r="K20" s="16">
+        <v>2</v>
+      </c>
+      <c r="L20" s="16">
+        <v>12</v>
+      </c>
+      <c r="M20" s="16">
+        <v>2</v>
+      </c>
+      <c r="N20" s="16">
         <v>1</v>
       </c>
-      <c r="G20" s="16">
-        <v>5</v>
-      </c>
-      <c r="H20" s="17">
-        <v>3</v>
-      </c>
-      <c r="I20" s="17">
-        <v>2</v>
-      </c>
-      <c r="J20" s="17">
-        <v>5</v>
-      </c>
-      <c r="K20" s="17">
-        <v>2</v>
-      </c>
-      <c r="L20" s="17">
-        <v>12</v>
-      </c>
-      <c r="M20" s="17">
-        <v>2</v>
-      </c>
-      <c r="N20" s="17">
+      <c r="O20" s="15">
+        <v>8</v>
+      </c>
+      <c r="P20" s="16">
+        <v>6</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>11</v>
+      </c>
+      <c r="R20" s="16">
+        <v>4</v>
+      </c>
+      <c r="S20" s="16">
+        <v>7</v>
+      </c>
+      <c r="T20" s="16">
+        <v>4</v>
+      </c>
+      <c r="U20" s="16">
         <v>1</v>
       </c>
-      <c r="O20" s="16">
-        <v>8</v>
-      </c>
-      <c r="P20" s="17">
-        <v>6</v>
-      </c>
-      <c r="Q20" s="17">
-        <v>11</v>
-      </c>
-      <c r="R20" s="17">
-        <v>4</v>
-      </c>
-      <c r="S20" s="17">
-        <v>7</v>
-      </c>
-      <c r="T20" s="17">
-        <v>4</v>
-      </c>
-      <c r="U20" s="17">
-        <v>1</v>
-      </c>
-      <c r="V20" s="18">
+      <c r="V20" s="17">
         <v>2</v>
       </c>
       <c r="W20" s="9">
@@ -8368,61 +8406,63 @@
       <c r="C21" s="10">
         <v>7</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="7">
         <v>7</v>
       </c>
       <c r="E21" s="10">
+        <f t="shared" si="6"/>
+        <v>0.875</v>
+      </c>
+      <c r="F21" s="28">
+        <f t="shared" si="7"/>
+        <v>0.875</v>
+      </c>
+      <c r="G21" s="15">
+        <v>9</v>
+      </c>
+      <c r="H21" s="16">
+        <v>9</v>
+      </c>
+      <c r="I21" s="16">
+        <v>8</v>
+      </c>
+      <c r="J21" s="16">
+        <v>6</v>
+      </c>
+      <c r="K21" s="16">
+        <v>3</v>
+      </c>
+      <c r="L21" s="16">
+        <v>4</v>
+      </c>
+      <c r="M21" s="16">
+        <v>3</v>
+      </c>
+      <c r="N21" s="16">
+        <v>3</v>
+      </c>
+      <c r="O21" s="15">
+        <v>3</v>
+      </c>
+      <c r="P21" s="16">
+        <v>9</v>
+      </c>
+      <c r="Q21" s="16">
+        <v>4</v>
+      </c>
+      <c r="R21" s="16">
+        <v>5</v>
+      </c>
+      <c r="S21" s="16">
+        <v>4</v>
+      </c>
+      <c r="T21" s="16">
+        <v>4</v>
+      </c>
+      <c r="U21" s="16">
         <v>1</v>
       </c>
-      <c r="F21" s="12">
-        <v>1</v>
-      </c>
-      <c r="G21" s="16">
-        <v>9</v>
-      </c>
-      <c r="H21" s="17">
-        <v>9</v>
-      </c>
-      <c r="I21" s="17">
-        <v>8</v>
-      </c>
-      <c r="J21" s="17">
-        <v>6</v>
-      </c>
-      <c r="K21" s="17">
-        <v>3</v>
-      </c>
-      <c r="L21" s="17">
-        <v>4</v>
-      </c>
-      <c r="M21" s="17">
-        <v>3</v>
-      </c>
-      <c r="N21" s="17">
-        <v>3</v>
-      </c>
-      <c r="O21" s="16">
-        <v>3</v>
-      </c>
-      <c r="P21" s="17">
-        <v>9</v>
-      </c>
-      <c r="Q21" s="17">
-        <v>4</v>
-      </c>
-      <c r="R21" s="17">
-        <v>5</v>
-      </c>
-      <c r="S21" s="17">
-        <v>4</v>
-      </c>
-      <c r="T21" s="17">
-        <v>4</v>
-      </c>
-      <c r="U21" s="17">
-        <v>1</v>
-      </c>
-      <c r="V21" s="18">
+      <c r="V21" s="17">
         <v>2</v>
       </c>
       <c r="W21" s="10">

</xml_diff>